<commit_message>
changing clustering and info organization scheme
</commit_message>
<xml_diff>
--- a/topic_split/topic_10.xlsx
+++ b/topic_split/topic_10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>issue</t>
   </si>
@@ -22,62 +22,42 @@
     <t>topic</t>
   </si>
   <si>
-    <t>confidence_score</t>
-  </si>
-  <si>
-    <t>[4.06057072e-308 2.34147746e-308 2.60847679e-308 2.22794007e-308
- 2.83094825e-308 3.51284144e-308 4.61185305e-308 3.58052244e-308
- 3.17684390e-308 1.00000000e+000 4.46804053e-308 3.20658625e-308
- 3.97571635e-308 2.89779182e-308 3.99778125e-308 1.91852310e-307
- 4.44658253e-308 4.10445265e-308 1.14800516e-307 1.42187436e-307
- 3.23148222e-308 6.61822135e-308 3.49444304e-308 2.62440630e-307
- 5.08300762e-308]</t>
-  </si>
-  <si>
-    <t>[4.04707945e-308 2.33964668e-308 2.59683223e-308 2.22643168e-308
- 2.81373293e-308 3.48608412e-308 4.56289572e-308 3.55008031e-308
- 3.15704617e-308 1.00000000e+000 4.42103650e-308 3.18931612e-308
- 3.94126167e-308 2.89142509e-308 3.96152588e-308 1.86648283e-307
- 4.40879275e-308 4.06842642e-308 1.11880939e-307 1.37415713e-307
- 3.21007135e-308 6.53317422e-308 3.46603790e-308 2.55241782e-307
- 5.03677374e-308]</t>
-  </si>
-  <si>
-    <t>[0.01031114 0.0058987  0.00629624 0.00562359 0.00683316 0.00871111
- 0.01171021 0.00893527 0.00767719 0.15080973 0.01088547 0.0076431
- 0.00989529 0.00733242 0.01018636 0.03544803 0.01113651 0.01059673
- 0.02512025 0.03447298 0.00785571 0.01651312 0.00859968 0.11608793
- 0.012024  ]</t>
-  </si>
-  <si>
-    <t>[0.01140111 0.00672367 0.00692123 0.00640167 0.00744528 0.00938567
- 0.01246313 0.00958854 0.0083689  0.15239091 0.01154422 0.0083654
- 0.01063125 0.00828847 0.01089309 0.03523536 0.01192456 0.01136301
- 0.02494632 0.03234679 0.00852515 0.017199   0.00924407 0.08396533
- 0.01286577]</t>
-  </si>
-  <si>
-    <t>[0.00705077 0.00411492 0.00443461 0.00391716 0.00478459 0.00597397
- 0.00788454 0.00609821 0.00538101 0.52387334 0.00749326 0.00541126
- 0.00676744 0.005084   0.00685823 0.02727041 0.00756977 0.00708024
- 0.01774183 0.02225266 0.005477   0.01110965 0.00592362 0.0509908
- 0.00846945]</t>
-  </si>
-  <si>
-    <t>[4.04962896e-308 2.35636153e-308 2.56611091e-308 2.24276199e-308
- 2.77221277e-308 3.45058815e-308 4.53813340e-308 3.51897319e-308
- 3.11577898e-308 1.00000000e+000 4.34493781e-308 3.13917354e-308
- 3.90186103e-308 2.91038392e-308 3.94599932e-308 1.66555995e-307
- 4.36811284e-308 4.06679692e-308 1.05089222e-307 1.30725230e-307
- 3.16897869e-308 6.42854826e-308 3.42319438e-308 2.76073135e-307
- 4.92583861e-308]</t>
-  </si>
-  <si>
-    <t>[0.01146437 0.00665305 0.0069244  0.00634238 0.00747426 0.00950104
- 0.01269348 0.00972774 0.00840099 0.14763277 0.01172921 0.00837074
- 0.01076782 0.00822912 0.01109763 0.03579184 0.01211173 0.01159137
- 0.02558988 0.03434261 0.00857897 0.01762602 0.00934684 0.10164532
- 0.01297032]</t>
+    <t>Kosovo label on the map
+We need to display 'Kosovo' on the map and also add a specific disclaimer.
+The typography should be somewhat lighter than the normal country names (e.g. font light version, or grey)
+![image](https://github.com/IFRCGo/go-frontend/assets/68283148/a111c27c-5303-42b7-b7bb-77646dfaedd6)
+The map disclaimer text:
+_The name and boundaries of Kosovo are consistent with [UN Security Council Resolution 1244](https://documents-dds-ny.un.org/doc/UNDOC/GEN/N99/172/89/PDF/N9917289.pdf?OpenElement) and the [ICJ's Advisory Opinion on the Unilateral Declaration of Independence in Respect of Kosovo](https://www.icj-cij.org/public/files/case-related/141/141-20100722-ADV-01-00-EN.pdf)._
+@frozenhelium, What are the display options for disclaimers? Can we show based on map view, zoom scale? Can we specify text in the disclaimer box based on the page url (e.g. showing it only on the map on the Serbia page)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PROD] Search result page - Ongoing Rapid response deployments section
+The search results page shows NOT ongoing deployments under the 'Ongoing rapid response deployments':
+![image](https://github.com/IFRCGo/go-frontend/assets/68283148/eacaad42-af72-49bb-862b-8f42ad01744d)
+There is an 'Ongoing' attribute of the deployments that should be used to filter deployments in this list.
+Similarly 'Open Surge Alerts' section should not how archived alerts:
+![image](https://github.com/IFRCGo/go-frontend/assets/68283148/9677c324-a2d2-4a2f-b748-4d07e14e70b4)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This hasn't been translated to any of the languages (https://go.ifrc.org/emergencies/6508#surge)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All appeals sorting
+When an user navigates to All Appeals https://go.ifrc.org/appeals/all?region=0 the records are sorted in a weird way, can we sort them by date? (With the most recent on top)
+![image](https://github.com/IFRCGo/go-infrastructure/assets/69478743/ac216540-dfcb-4044-a321-5aaf7dcc62c0)
+@szabozoltan69 @tovari </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PROD] Embedded content appears only partially on Region pages
+There is an embedded dashboard on the APAC region page that isn't show up correctly on the frontend.
+https://go.ifrc.org/regions/2/additional-info
+![Image](https://github.com/user-attachments/assets/d1227f33-5739-46e1-8a92-3b00745a752d)
+It seems, all is okay on the admin page, the snippet Preview shows it also correctly:
+https://goadmin.ifrc.org/en/admin/api/region/2/change/
+![Image](https://github.com/user-attachments/assets/f6785bb3-603e-42a0-b615-65169419329f)
+</t>
   </si>
 </sst>
 </file>
@@ -435,97 +415,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>180</v>
       </c>
       <c r="B2">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>184</v>
       </c>
       <c r="B3">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>185</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>186</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>188</v>
-      </c>
       <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>189</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>193</v>
-      </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>